<commit_message>
Bug Fix Feature import Guru Mapel
</commit_message>
<xml_diff>
--- a/public/excel/template-guru-mapel.xlsx
+++ b/public/excel/template-guru-mapel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ketuntasan\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355BCD9A-2734-4C06-B158-9DFB85A4F730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1296DB1-6544-4AB9-B75C-72DA15F292B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{61C89190-9635-4525-9D08-AA1415C04976}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{61C89190-9635-4525-9D08-AA1415C04976}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <r>
       <t xml:space="preserve">SILAHKAN MASUKKAN
@@ -93,9 +90,6 @@
 SILAHKAN MASUKKAN KODE GURU
 DI DALAM SYMBOL [ ]</t>
     </r>
-  </si>
-  <si>
-    <t>[1]</t>
   </si>
   <si>
     <t>[2]</t>
@@ -128,6 +122,12 @@
 DI DALAM SYMBOL [ ]
 APABILA LEBIH DARI 1 MAPEL PISAHKAN DENGAN PETIK SATU '</t>
     </r>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
+    <t>[4]</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +533,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -546,18 +546,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug Fix All Features in Role Superadmin,Siswa,Guru
</commit_message>
<xml_diff>
--- a/public/excel/template-guru-mapel.xlsx
+++ b/public/excel/template-guru-mapel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ketuntasan\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1296DB1-6544-4AB9-B75C-72DA15F292B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4627049-6E68-4FEC-A2B6-634AA12D2E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{61C89190-9635-4525-9D08-AA1415C04976}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <r>
       <t xml:space="preserve">SILAHKAN MASUKKAN
@@ -66,75 +66,12 @@
       <t>KODE MAPEL</t>
     </r>
   </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PETUNJUK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-SILAHKAN MASUKKAN KODE GURU
-DI DALAM SYMBOL [ ]</t>
-    </r>
-  </si>
-  <si>
-    <t>[2]</t>
-  </si>
-  <si>
-    <t>[1'2'3]</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PETUNJUK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-SILAHKAN MASUKKAN KODE MAPEL
-DI DALAM SYMBOL [ ]
-APABILA LEBIH DARI 1 MAPEL PISAHKAN DENGAN PETIK SATU '</t>
-    </r>
-  </si>
-  <si>
-    <t>[3]</t>
-  </si>
-  <si>
-    <t>[4]</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,16 +87,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,12 +98,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -191,15 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -516,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE3E785-8899-4F01-9EC6-AF653FB893E6}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,36 +449,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6"/>
+      <c r="B6"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7"/>
+      <c r="B7"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8"/>
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9"/>
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10"/>
+      <c r="B10"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11"/>
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12"/>
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13"/>
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14"/>
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15"/>
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16"/>
+      <c r="B16"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17"/>
+      <c r="B17"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18"/>
+      <c r="B18"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19"/>
+      <c r="B19"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20"/>
+      <c r="B20"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21"/>
+      <c r="B21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>